<commit_message>
update sectoral data breakdown to include EIU index
</commit_message>
<xml_diff>
--- a/data_raw/indices_sector.xlsx
+++ b/data_raw/indices_sector.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaon\OneDrive\Courses\201901\GOV282\Group Project\freedomhouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaon\OneDrive\Courses\201901\GOV282\Group Project\freedomhouse\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3036FC04-D0FB-45C3-9FA7-00D90832FC7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AF09B40C-59F0-40CB-8DD3-3D32BA952353}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D86BFC9-E5E0-4A65-8AC5-C0AFB1A8F3D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8935" yWindow="2055" windowWidth="9600" windowHeight="7180" xr2:uid="{0F823799-FF00-43C9-92C1-4576B0D05852}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{0F823799-FF00-43C9-92C1-4576B0D05852}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>sector</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>mentions</t>
+  </si>
+  <si>
+    <t>EIU</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2FE4A6-AAA9-451A-B71A-7F322F227E78}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -494,6 +497,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3580</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>